<commit_message>
Add CRUD API for applications with FastAPI
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -1286,8 +1286,8 @@
   <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>

</xml_diff>